<commit_message>
updated rookie survival info
</commit_message>
<xml_diff>
--- a/rookie survival.xlsx
+++ b/rookie survival.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rookie_survival" sheetId="1" r:id="rId1"/>
     <sheet name="Raw Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -2008,7 +2008,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -2026,7 +2026,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <font>
@@ -2045,26 +2045,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <font>
@@ -2121,7 +2102,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2159,6 +2140,25 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
@@ -2178,7 +2178,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2235,26 +2235,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2291,19 +2271,19 @@
     <tableColumn id="7" name="&gt;= 4" dataDxfId="10">
       <calculatedColumnFormula>COUNTIFS(Table1[rookie year],Table2[[#This Row],[Rookie Year]],Table1['# active years],"&gt;=4")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="% never played" dataDxfId="9" totalsRowDxfId="0" dataCellStyle="Percent">
+    <tableColumn id="8" name="% never played" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[Never played]]/Table2[[#This Row],['# of teams]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="% at least 1 year" dataDxfId="8" totalsRowDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="9" name="% at least 1 year" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[&gt;= 1]]/Table2[[#This Row],['# of teams]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="% at least 2 years" dataDxfId="7" totalsRowDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="10" name="% at least 2 years" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[&gt;= 2]]/Table2[[#This Row],['# of teams]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="% at least 3 years" dataDxfId="6" totalsRowDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="11" name="% at least 3 years" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[&gt;= 3]]/Table2[[#This Row],['# of teams]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="% at least 4 years" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="12" name="% at least 4 years" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Percent">
       <calculatedColumnFormula>Table2[[#This Row],[&gt;= 4]]/Table2[[#This Row],['# of teams]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2623,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3856,6 +3836,28 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>rookie_survival!I2:L2</xm:f>
+              <xm:sqref>N2</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3863,7 +3865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5391"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>